<commit_message>
change CORRES to AUTHOR
</commit_message>
<xml_diff>
--- a/subsidiary_doc/notKnowingAffiliations.xlsx
+++ b/subsidiary_doc/notKnowingAffiliations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="600" yWindow="150" windowWidth="20115" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Affiliations that cannot find the identifier in Pure</t>
   </si>
@@ -194,6 +194,179 @@
   </si>
   <si>
     <r>
+      <t>Department of Chemical Engineering,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> University of Washington</t>
+    </r>
+  </si>
+  <si>
+    <t>State Academy of Art and Design</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">High Resolution Powder Diffraction Beamline (I11), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diamond Light Source Ltd</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Max Planck Institute of Colloids and Interfaces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Department of Colloid Chemistry, Research Campus Golm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Institute of Microtechnology, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TU Braunschweig</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Department of Materials Science and Engineering, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Norwegian University of Science and Technology</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Secció de Fisicoquímica, Facultat de Farmàcia i Ciències de l'Alimentació, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Universitat de Barcelona</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Grupo de Física de Fluidos y Biocoloides, Departamento de Física Aplicada, Facultad de Ciencias, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Universidad de Granada</t>
+    </r>
+  </si>
+  <si>
+    <t>Max Planck Institute for the Physics of Complex Systems</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IRIDIA, CoDE, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Université libre de Bruxelles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Department of Physics,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Institute for Advanced Studies in Basic Sciences (IASBS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Department of Physics, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alzahra University</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Max Planck Institute for </t>
     </r>
     <r>
@@ -205,7 +378,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Terrestrial Microbiology and LOEWE Center for Synthetic Microbiology</t>
+      <t>Terrestrial Microbiology</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and LOEWE Center for Synthetic Microbiology</t>
     </r>
     <r>
       <rPr>
@@ -219,184 +403,20 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Department of Chemical Engineering,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> University of Washington</t>
-    </r>
-  </si>
-  <si>
-    <t>State Academy of Art and Design</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">High Resolution Powder Diffraction Beamline (I11), </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Diamond Light Source Ltd</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Max Planck Institute of Colloids and Interfaces</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, Department of Colloid Chemistry, Research Campus Golm</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Institute of Microtechnology, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TU Braunschweig</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Department of Materials Science and Engineering, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Norwegian University of Science and Technology</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Secció de Fisicoquímica, Facultat de Farmàcia i Ciències de l'Alimentació, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Universitat de Barcelona</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Grupo de Física de Fluidos y Biocoloides, Departamento de Física Aplicada, Facultad de Ciencias, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Universidad de Granada</t>
-    </r>
-  </si>
-  <si>
-    <t>Max Planck Institute for the Physics of Complex Systems</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">IRIDIA, CoDE, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Université libre de Bruxelles</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Department of Physics,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Institute for Advanced Studies in Basic Sciences (IASBS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Department of Physics, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alzahra University</t>
-    </r>
+    <t>ou_1863284</t>
+  </si>
+  <si>
+    <t>ou_2117288</t>
+  </si>
+  <si>
+    <t>ou_persistent22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +428,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -742,32 +770,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -775,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -783,7 +815,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -791,93 +823,99 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="75" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>